<commit_message>
updated some android build files | updated Planung | Fixed Plakate
</commit_message>
<xml_diff>
--- a/Planung.xlsx
+++ b/Planung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgaben" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Projektname</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>Aufgabenliste</t>
+  </si>
+  <si>
+    <t>Karteikarten erstellen</t>
+  </si>
+  <si>
+    <t>Vortrag anpassen &amp; neu zuweisen</t>
+  </si>
+  <si>
+    <t>nicht Begonnen</t>
   </si>
 </sst>
 </file>
@@ -363,7 +372,132 @@
     <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -761,10 +895,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Liste &quot;Gruppenprojekt&quot;" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Liste &quot;Gruppenprojekt&quot;" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="52"/>
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="totalRow" dxfId="50"/>
-      <tableStyleElement type="firstColumn" dxfId="49"/>
+      <tableStyleElement type="wholeTable" dxfId="69"/>
+      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="totalRow" dxfId="67"/>
+      <tableStyleElement type="firstColumn" dxfId="66"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -784,18 +918,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="B6:G14" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B6:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="B7:G14">
-    <sortCondition descending="1" ref="F6:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="B6:G16" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="B6:G16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="B7:G16">
+    <sortCondition descending="1" ref="F6:F16"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Zuständiger" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priorität" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Zieldatum" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Notizen" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Zuständiger" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priorität" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Zieldatum" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Notizen" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="Liste &quot;Gruppenprojekt&quot;" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1073,10 +1207,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G14"/>
+  <dimension ref="B1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1151,199 +1285,233 @@
     </row>
     <row r="7" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>43125</v>
+        <v>43143</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2">
-        <v>43154</v>
+        <v>43143</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2">
-        <v>43133</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="13"/>
+        <v>43125</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2">
-        <v>43130</v>
-      </c>
-      <c r="F10" s="16" t="s">
+        <v>43154</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="12">
-        <v>43129</v>
+      <c r="E11" s="2">
+        <v>43133</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2">
-        <v>43114</v>
+        <v>43130</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="2">
-        <v>43116</v>
+      <c r="E13" s="12">
+        <v>43129</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>19</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2">
+        <v>43114</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <v>43116</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E16" s="2">
         <v>43138</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F13 F11">
-    <cfRule type="expression" dxfId="48" priority="52">
+    <cfRule type="expression" dxfId="65" priority="69">
       <formula>UPPER(F11)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="53">
+    <cfRule type="expression" dxfId="64" priority="70">
       <formula>UPPER(F11)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="54">
+    <cfRule type="expression" dxfId="63" priority="71">
       <formula>UPPER(F11)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="niedrig">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="niedrig">
       <formula>NOT(ISERROR(SEARCH("niedrig",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="61" priority="61" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12 D7:D8">
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="mittel">
+    <cfRule type="containsText" dxfId="59" priority="59" operator="containsText" text="mittel">
       <formula>NOT(ISERROR(SEARCH("mittel",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="hoch">
+    <cfRule type="containsText" dxfId="58" priority="58" operator="containsText" text="hoch">
       <formula>NOT(ISERROR(SEARCH("hoch",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="containsText" dxfId="40" priority="64" operator="containsText" text="mittel">
+    <cfRule type="containsText" dxfId="57" priority="81" operator="containsText" text="mittel">
       <formula>NOT(ISERROR(SEARCH("mittel",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="65" operator="containsText" text="hoch">
+    <cfRule type="containsText" dxfId="56" priority="82" operator="containsText" text="hoch">
       <formula>NOT(ISERROR(SEARCH("hoch",D11)))</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1355,127 +1523,185 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="55" priority="55">
       <formula>UPPER(F9)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="54" priority="56">
       <formula>UPPER(F9)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="40">
+    <cfRule type="expression" dxfId="53" priority="57">
       <formula>UPPER(F9)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="33" priority="30">
+    <cfRule type="expression" dxfId="50" priority="47">
       <formula>UPPER(F12)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="31">
+    <cfRule type="expression" dxfId="49" priority="48">
       <formula>UPPER(F12)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="48" priority="49">
       <formula>UPPER(F12)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="30" priority="27">
+    <cfRule type="expression" dxfId="47" priority="44">
       <formula>UPPER(F10)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="46" priority="45">
       <formula>UPPER(F10)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="45" priority="46">
       <formula>UPPER(F10)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="27" priority="26" operator="containsText" text="niedrig">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="niedrig">
       <formula>NOT(ISERROR(SEARCH("niedrig",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="mittel">
+    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="mittel">
       <formula>NOT(ISERROR(SEARCH("mittel",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="25" priority="22">
+    <cfRule type="expression" dxfId="42" priority="39">
       <formula>UPPER(F8)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="23">
+    <cfRule type="expression" dxfId="41" priority="40">
       <formula>UPPER(F8)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula>UPPER(F8)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="22" priority="16">
+    <cfRule type="expression" dxfId="39" priority="33">
       <formula>UPPER(F7)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="17">
+    <cfRule type="expression" dxfId="38" priority="34">
       <formula>UPPER(F7)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="37" priority="35">
       <formula>UPPER(F7)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="36" priority="31" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="35" priority="32" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="34" priority="27" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="33" priority="28" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="32" priority="25" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="28" priority="20">
       <formula>UPPER(F14)="nicht begonnen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="27" priority="21">
       <formula>UPPER(F14)="in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="26" priority="22">
       <formula>UPPER(F14)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Vincent">
+    <cfRule type="containsText" dxfId="25" priority="18" operator="containsText" text="Vincent">
       <formula>NOT(ISERROR(SEARCH("Vincent",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Fabian">
+    <cfRule type="containsText" dxfId="24" priority="19" operator="containsText" text="Fabian">
       <formula>NOT(ISERROR(SEARCH("Fabian",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Vincent">
+      <formula>NOT(ISERROR(SEARCH("Vincent",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Fabian">
+      <formula>NOT(ISERROR(SEARCH("Fabian",C15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Vincent">
+      <formula>NOT(ISERROR(SEARCH("Vincent",C16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Fabian">
+      <formula>NOT(ISERROR(SEARCH("Fabian",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="niedrig">
+      <formula>NOT(ISERROR(SEARCH("niedrig",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="mittel">
+      <formula>NOT(ISERROR(SEARCH("mittel",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="niedrig">
+      <formula>NOT(ISERROR(SEARCH("niedrig",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="mittel">
+      <formula>NOT(ISERROR(SEARCH("mittel",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>UPPER(F15)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>UPPER(F15)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>UPPER(F15)="erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>UPPER(F16)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>UPPER(F16)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>UPPER(F16)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>